<commit_message>
made different files for the link sharing and calling
</commit_message>
<xml_diff>
--- a/Sales_Conversation.xlsx
+++ b/Sales_Conversation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -817,6 +817,141 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>smart watch</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2025-10-31 12:56:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us.</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2025-10-31 12:56:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>laptop</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2025-10-31 12:59:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2025-10-31 13:00:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us.</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2025-10-31 13:00:36</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
created a new funnel for lead gathering and link sharing funnel
</commit_message>
<xml_diff>
--- a/Sales_Conversation.xlsx
+++ b/Sales_Conversation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -952,6 +952,60 @@
         </is>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>I totally understand! But just to let you know, we have a special offer running — a 20% discount on all products today only! Would you like me to show you some options?</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>2025-10-31 16:23:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>User rejected offer after persuasion</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>2025-10-31 16:23:50</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
implemented the sms service by tripada in the speech link sharing
</commit_message>
<xml_diff>
--- a/Sales_Conversation.xlsx
+++ b/Sales_Conversation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1006,6 +1006,195 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>earbuds</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>2025-10-31 18:56:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us.Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>2025-10-31 18:57:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us.Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>2025-10-31 19:00:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2025-10-31 19:13:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>2025-10-31 19:22:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>2025-10-31 19:34:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 0234. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>2025-10-31 19:39:39</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Improved speed of the bot optimise working,Improved bot listing to user response,Can recognise easy
</commit_message>
<xml_diff>
--- a/Sales_Conversation.xlsx
+++ b/Sales_Conversation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1195,6 +1195,972 @@
         </is>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:16:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>not interested</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals? </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:16:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>I hear you! However, we’ve got a limited-time combo offer where you can save even more. Would you like to check that out?</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:16:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Alright! But trust me, this week’s festive sale is really something special — 25% off on bestsellers! Interested?</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:17:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Okay, I get it. Still, let me tell you — even browsing our collection could give you an idea for your next purchase. Shall I share a link?</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:17:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>No problem at all! But just one last thing — we’re giving exclusive coupons for early customers today. Should I send one to you?</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:18:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>No problem at all! But just one last thing — we’re giving exclusive coupons for early customers today. Should I send one to you?</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:18:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>No problem at all! But just one last thing — we’re giving exclusive coupons for early customers today. Should I send one to you?</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:18:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>No problem at all! But just one last thing — we’re giving exclusive coupons for early customers today. Should I send one to you?</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:19:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>sure</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>User rejected offer after persuasion</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:19:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>not interested</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:25:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals? </t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:25:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>yes please go ahead</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>User rejected offer after persuasion</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>2025-11-01 12:25:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals?</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:00:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>I hear you! However, we’ve got a limited-time combo offer where you can save even more. Would you like to check that out?</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:01:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>go ahead yes please go ahead</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:01:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Bluetooth earbud</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:02:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 7606. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:02:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:32:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals?</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:32:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>I hear you! However, we’ve got a limited-time combo offer where you can save even more. Would you like to check that out?</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:33:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>yes please</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:33:37</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 7606. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>2025-11-01 13:34:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:45:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>no</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Totally fair! But if I may — we’re offering free delivery on all products this week. Can I share a few top deals?</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:45:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>I hear you! However, we’ve got a limited-time combo offer where you can save even more. Would you like to check that out?</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:45:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>I said yes please go ahead</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:46:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>speaker</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Product not found. Shown offers again.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:47:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>No response</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>I completely understand! But before you go — we’re giving a 20% discount just for today. Would you like to take a quick look?</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:47:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>bluetooth speaker Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 7606. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:48:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>bluetooth speaker Bluetooth earbuds</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2025-11-01 15:48:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>sure</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>happy</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Here are our latest offers:
+- Laptop Pro 
+- Smart watch 
+- Bluetooth Earbuds
+Which product would you like to purchase?</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:04:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Bluetooth</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Bluetooth Earbuds to your phone number ending with 7606. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:05:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Bluetooth</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2025-11-01 16:05:44</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
implemented the agent calling thing in particular time in speechlinkshare if the user has requested and in leadGathering made optimise and faster little bit
</commit_message>
<xml_diff>
--- a/Sales_Conversation.xlsx
+++ b/Sales_Conversation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2161,6 +2161,200 @@
         </is>
       </c>
     </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Talk to agent requested (after hours)</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Our agent will contact you later.</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:04:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Asked about products after call request</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Asked user if they want to hear about products after call request.</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:04:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>to agent</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Product not found. Shown offers again.
+Here are our latest offers:
+- Laptop Pro : one of the best laptop you can get right now with high end specs at ₹75000
+- Smart watch : Best watch in market with all your daily tracking at ₹12000
+- Bluetooth Earbuds: best anc earbuds with this price point  at ₹4000
+</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:05:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Talk to agent requested (after hours)</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Our agent will contact you later.</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:05:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Asked about products after call request</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Asked user if they want to hear about products after call request.</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:05:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>laptop</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Great choice! I’ve sent the link of Laptop Pro  to your phone number ending with 7606. Thank you for your time! I really appreciate it. If you need anything, feel free to contact us. Our Contact number is 20251.</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:06:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Hi there! I’m your sales agent from Creer Infotech. I’ve reached out to share some exciting offers on our latest products. Can I take a few minutes to tell you about them?</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>laptop</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>I'm sorry, I didn’t catch that.</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>2025-11-01 17:06:20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>